<commit_message>
Gráfica de columnas apiladas de población
</commit_message>
<xml_diff>
--- a/08/GraficosII.xlsx
+++ b/08/GraficosII.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Iris" sheetId="1" r:id="rId1"/>
     <sheet name="Datos discretos" sheetId="2" r:id="rId2"/>
     <sheet name="Valores continuos" sheetId="3" r:id="rId3"/>
     <sheet name="Valores acumulados" sheetId="4" r:id="rId4"/>
+    <sheet name="ColumnasApiladas" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="23">
   <si>
     <t>Sepal.Length</t>
   </si>
@@ -87,6 +88,15 @@
   </si>
   <si>
     <t>Población mundial</t>
+  </si>
+  <si>
+    <t>País</t>
+  </si>
+  <si>
+    <t>Rural</t>
+  </si>
+  <si>
+    <t>Urbana</t>
   </si>
 </sst>
 </file>
@@ -160,10 +170,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
@@ -3613,6 +3629,492 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Población rural/urbana</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ColumnasApiladas!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rural</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ColumnasApiladas!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>  Australia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>  Papua Nueva Guinea</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>  Nueva Zelandia</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>  Fiji, Islas</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>  Salomón, Islas</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>  Polinesia Francesa</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>  Nueva Caledonia</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>  Vanuatu</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>  Samoa</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>  Guam</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ColumnasApiladas!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2863</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3897</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>348</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4EA1-4A95-ADC1-638A4AC5537A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ColumnasApiladas!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Urbana</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ColumnasApiladas!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>  Australia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>  Papua Nueva Guinea</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>  Nueva Zelandia</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>  Fiji, Islas</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>  Salomón, Islas</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>  Polinesia Francesa</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>  Nueva Caledonia</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>  Vanuatu</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>  Samoa</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>  Guam</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ColumnasApiladas!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0" formatCode="#,##0">
+                  <c:v>15838</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>806</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="#,##0">
+                  <c:v>3320</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4EA1-4A95-ADC1-638A4AC5537A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="756289888"/>
+        <c:axId val="756285624"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="756289888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="756285624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="756285624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="756289888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -3810,6 +4312,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6255,6 +6797,511 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -6518,6 +7565,41 @@
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>242886</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9477,242 +10559,242 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="2">
+      <c r="A24" s="4">
         <v>42418</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="5">
         <v>1.1084000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="4">
+      <c r="A25" s="6">
         <v>42417</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="7">
         <v>1.1135999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="2">
+      <c r="A26" s="4">
         <v>42416</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="5">
         <v>1.1166</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="4">
+      <c r="A27" s="6">
         <v>42415</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="7">
         <v>1.1180000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="2">
+      <c r="A28" s="4">
         <v>42412</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="5">
         <v>1.1274999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="4">
+      <c r="A29" s="6">
         <v>42411</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="7">
         <v>1.1347</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="2">
+      <c r="A30" s="4">
         <v>42410</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="5">
         <v>1.1256999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="4">
+      <c r="A31" s="6">
         <v>42409</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="7">
         <v>1.1235999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="2">
+      <c r="A32" s="4">
         <v>42408</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="5">
         <v>1.1101000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="4">
+      <c r="A33" s="6">
         <v>42405</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="7">
         <v>1.1202000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="2">
+      <c r="A34" s="4">
         <v>42404</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="5">
         <v>1.1206</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="4">
+      <c r="A35" s="6">
         <v>42403</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="7">
         <v>1.0932999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="2">
+      <c r="A36" s="4">
         <v>42402</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="5">
         <v>1.0919000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="4">
+      <c r="A37" s="6">
         <v>42401</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="7">
         <v>1.0884</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="2">
+      <c r="A38" s="4">
         <v>42398</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="5">
         <v>1.0920000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="4">
+      <c r="A39" s="6">
         <v>42397</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="7">
         <v>1.0903</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="2">
+      <c r="A40" s="4">
         <v>42396</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="5">
         <v>1.0888</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="4">
+      <c r="A41" s="6">
         <v>42395</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="7">
         <v>1.0837000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="2">
+      <c r="A42" s="4">
         <v>42394</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="5">
         <v>1.0814999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="4">
+      <c r="A43" s="6">
         <v>42391</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="7">
         <v>1.0808</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="2">
+      <c r="A44" s="4">
         <v>42390</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="5">
         <v>1.0892999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="4">
+      <c r="A45" s="6">
         <v>42389</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="7">
         <v>1.0907</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="2">
+      <c r="A46" s="4">
         <v>42388</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="5">
         <v>1.0868</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="4">
+      <c r="A47" s="6">
         <v>42387</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="7">
         <v>1.0891999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="2">
+      <c r="A48" s="4">
         <v>42384</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="5">
         <v>1.0913999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="4">
+      <c r="A49" s="6">
         <v>42383</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="7">
         <v>1.0892999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="2">
+      <c r="A50" s="4">
         <v>42382</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="5">
         <v>1.0815999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="4">
+      <c r="A51" s="6">
         <v>42381</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="7">
         <v>1.0835999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="2">
+      <c r="A52" s="4">
         <v>42380</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="5">
         <v>1.0888</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A53" s="6">
+      <c r="A53" s="8">
         <v>42377</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="9">
         <v>1.0861000000000001</v>
       </c>
     </row>
@@ -9737,194 +10819,194 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="8">
+      <c r="A1" s="10">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B1" s="9">
+      <c r="B1" s="11">
         <v>10.199999999999999</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="8">
+      <c r="A2" s="10">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="11">
         <v>8.6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="8">
+      <c r="A3" s="10">
         <v>0.375</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="11">
         <v>7.9</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="8">
+      <c r="A4" s="10">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="11">
         <v>7.5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="8">
+      <c r="A5" s="10">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="11">
         <v>7.6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="8">
+      <c r="A6" s="10">
         <v>0.25</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="11">
         <v>5.3</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="8">
+      <c r="A7" s="10">
         <v>0.20833333333333334</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="11">
         <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="8">
+      <c r="A8" s="10">
         <v>0.16666666666666666</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="11">
         <v>6.5</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="8">
+      <c r="A9" s="10">
         <v>0.125</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="11">
         <v>5.6</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="8">
+      <c r="A10" s="10">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="11">
         <v>5.9</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="8">
+      <c r="A11" s="10">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="11">
         <v>6.1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="8">
+      <c r="A12" s="10">
         <v>0</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="11">
         <v>6.2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="8">
+      <c r="A13" s="10">
         <v>0.95833333333333337</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="11">
         <v>6.4</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="8">
+      <c r="A14" s="10">
         <v>0.91666666666666663</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="11">
         <v>6.3</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="8">
+      <c r="A15" s="10">
         <v>0.875</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="11">
         <v>6.3</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="8">
+      <c r="A16" s="10">
         <v>0.83333333333333337</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="11">
         <v>6.2</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="8">
+      <c r="A17" s="10">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="11">
         <v>6.3</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="8">
+      <c r="A18" s="10">
         <v>0.75</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="11">
         <v>6.5</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="8">
+      <c r="A19" s="10">
         <v>0.70833333333333337</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="11">
         <v>6.5</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="8">
+      <c r="A20" s="10">
         <v>0.66666666666666663</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="11">
         <v>6.4</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="8">
+      <c r="A21" s="10">
         <v>0.625</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="11">
         <v>6.3</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="8">
+      <c r="A22" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="11">
         <v>6.2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="8">
+      <c r="A23" s="10">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="11">
         <v>5.8</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="8">
+      <c r="A24" s="10">
         <v>0.5</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="11">
         <v>5.3</v>
       </c>
     </row>
@@ -9938,178 +11020,315 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="11">
+      <c r="A2" s="13">
         <v>1000</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="13">
         <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="11">
+      <c r="A3" s="13">
         <v>1650</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="13">
         <v>545</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="11">
+      <c r="A4" s="13">
         <v>1750</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="13">
         <v>791</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="11">
+      <c r="A5" s="13">
         <v>1800</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="13">
         <v>981</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="11">
+      <c r="A6" s="13">
         <v>1850</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="14">
         <v>1262</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="11">
+      <c r="A7" s="13">
         <v>1900</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="14">
         <v>1650</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="11">
+      <c r="A8" s="13">
         <v>1950</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="14">
         <v>2516</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="11">
+      <c r="A9" s="13">
         <v>1955</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="14">
         <v>2751</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="11">
+      <c r="A10" s="13">
         <v>1960</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="14">
         <v>3018</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="11">
+      <c r="A11" s="13">
         <v>1965</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="14">
         <v>3335</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="11">
+      <c r="A12" s="13">
         <v>1970</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="14">
         <v>3697</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="11">
+      <c r="A13" s="13">
         <v>1975</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="14">
         <v>4077</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="11">
+      <c r="A14" s="13">
         <v>1980</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="14">
         <v>4446</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="11">
+      <c r="A15" s="13">
         <v>1985</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="14">
         <v>4854</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="11">
+      <c r="A16" s="13">
         <v>1990</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="14">
         <v>5259</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="11">
+      <c r="A17" s="13">
         <v>1995</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="14">
         <v>5759</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="11">
+      <c r="A18" s="13">
         <v>2000</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="14">
         <v>6228</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="11">
+      <c r="A19" s="13">
         <v>2005</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="14">
         <v>6574</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="13">
+      <c r="A20" s="15">
         <v>2010</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="16">
         <v>6894</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="13">
+      <c r="A21" s="15">
         <v>2015</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="16">
         <v>7349</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2863</v>
+      </c>
+      <c r="C2" s="2">
+        <v>15838</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3897</v>
+      </c>
+      <c r="C3" s="3">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3">
+        <v>509</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3">
+        <v>468</v>
+      </c>
+      <c r="C5" s="3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3">
+        <v>348</v>
+      </c>
+      <c r="C6" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3">
+        <v>100</v>
+      </c>
+      <c r="C7" s="3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3">
+        <v>76</v>
+      </c>
+      <c r="C8" s="3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3">
+        <v>149</v>
+      </c>
+      <c r="C9" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3">
+        <v>139</v>
+      </c>
+      <c r="C10" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3">
+        <v>100</v>
+      </c>
+      <c r="C11" s="3">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hoja con gráficas de columna apiladas
</commit_message>
<xml_diff>
--- a/08/GraficosII.xlsx
+++ b/08/GraficosII.xlsx
@@ -19,6 +19,7 @@
     <sheet name="ColumnasApiladas" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -221,8 +222,36 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1785,6 +1814,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-3736-4D2F-8799-49713E2EC095}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1799,6 +1833,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-3736-4D2F-8799-49713E2EC095}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1813,6 +1852,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-3736-4D2F-8799-49713E2EC095}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1827,6 +1871,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-3736-4D2F-8799-49713E2EC095}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1841,6 +1890,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-3736-4D2F-8799-49713E2EC095}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1855,6 +1909,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-3736-4D2F-8799-49713E2EC095}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -1871,6 +1930,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-3736-4D2F-8799-49713E2EC095}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -1887,6 +1951,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-3736-4D2F-8799-49713E2EC095}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -1903,6 +1972,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-3736-4D2F-8799-49713E2EC095}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -1919,6 +1993,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-3736-4D2F-8799-49713E2EC095}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -4115,6 +4194,492 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Población rural/urbana</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ColumnasApiladas!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rural</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ColumnasApiladas!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>  Australia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>  Papua Nueva Guinea</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>  Nueva Zelandia</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>  Fiji, Islas</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>  Salomón, Islas</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>  Polinesia Francesa</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>  Nueva Caledonia</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>  Vanuatu</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>  Samoa</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>  Guam</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ColumnasApiladas!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2863</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3897</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>348</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-67A8-4054-AC07-E5B863E1C0F1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ColumnasApiladas!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Urbana</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>ColumnasApiladas!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>  Australia</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>  Papua Nueva Guinea</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>  Nueva Zelandia</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>  Fiji, Islas</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>  Salomón, Islas</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>  Polinesia Francesa</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>  Nueva Caledonia</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>  Vanuatu</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>  Samoa</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>  Guam</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ColumnasApiladas!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0" formatCode="#,##0">
+                  <c:v>15838</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>806</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="#,##0">
+                  <c:v>3320</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-67A8-4054-AC07-E5B863E1C0F1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="576441248"/>
+        <c:axId val="576442560"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="576441248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="576442560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="576442560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="576441248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -4352,6 +4917,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6912,6 +7517,511 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7613,6 +8723,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>176211</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11205,7 +12345,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Hoja con gráfica de tarta
</commit_message>
<xml_diff>
--- a/08/GraficosII.xlsx
+++ b/08/GraficosII.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Iris" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Valores continuos" sheetId="3" r:id="rId3"/>
     <sheet name="Valores acumulados" sheetId="4" r:id="rId4"/>
     <sheet name="ColumnasApiladas" sheetId="5" r:id="rId5"/>
+    <sheet name="Proporciones" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="32">
   <si>
     <t>Sepal.Length</t>
   </si>
@@ -98,6 +99,33 @@
   </si>
   <si>
     <t>Urbana</t>
+  </si>
+  <si>
+    <t>África</t>
+  </si>
+  <si>
+    <t>Continente</t>
+  </si>
+  <si>
+    <t>Hombres</t>
+  </si>
+  <si>
+    <t>Mujeres</t>
+  </si>
+  <si>
+    <t>América</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>Europa</t>
+  </si>
+  <si>
+    <t>Oceanía</t>
+  </si>
+  <si>
+    <t>Población</t>
   </si>
 </sst>
 </file>
@@ -4680,6 +4708,609 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Proporciones!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Población</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="10000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="127000" h="127000"/>
+                <a:bevelB w="127000" h="127000"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-B3A8-45EC-9F7C-11E72BD1D92E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="10000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="127000" h="127000"/>
+                <a:bevelB w="127000" h="127000"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-B3A8-45EC-9F7C-11E72BD1D92E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="10000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="127000" h="127000"/>
+                <a:bevelB w="127000" h="127000"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-B3A8-45EC-9F7C-11E72BD1D92E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="10000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="127000" h="127000"/>
+                <a:bevelB w="127000" h="127000"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-B3A8-45EC-9F7C-11E72BD1D92E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="10000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d>
+                <a:bevelT w="127000" h="127000"/>
+                <a:bevelB w="127000" h="127000"/>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-B3A8-45EC-9F7C-11E72BD1D92E}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent1"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-B3A8-45EC-9F7C-11E72BD1D92E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-B3A8-45EC-9F7C-11E72BD1D92E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-B3A8-45EC-9F7C-11E72BD1D92E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-B3A8-45EC-9F7C-11E72BD1D92E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-B3A8-45EC-9F7C-11E72BD1D92E}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Proporciones!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>África</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>América</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Asia</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Europa</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Oceanía</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Proporciones!$F$2:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>766621</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>818445</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3634280</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>739508</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B3A8-45EC-9F7C-11E72BD1D92E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -4957,6 +5588,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8460,6 +9131,526 @@
           <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="259">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="auto"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="10000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d>
+        <a:bevelT w="127000" h="127000"/>
+        <a:bevelB w="127000" h="127000"/>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -8761,6 +9952,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>414337</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -12344,7 +13570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -12475,4 +13701,140 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>381985</v>
+      </c>
+      <c r="C2">
+        <v>384409</v>
+      </c>
+      <c r="D2">
+        <v>482608</v>
+      </c>
+      <c r="E2">
+        <v>284013</v>
+      </c>
+      <c r="F2">
+        <v>766621</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>404328</v>
+      </c>
+      <c r="C3">
+        <v>413098</v>
+      </c>
+      <c r="D3">
+        <v>198578</v>
+      </c>
+      <c r="E3">
+        <v>619867</v>
+      </c>
+      <c r="F3">
+        <v>818445</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>1857046</v>
+      </c>
+      <c r="C4">
+        <v>1777230</v>
+      </c>
+      <c r="D4">
+        <v>2291330</v>
+      </c>
+      <c r="E4">
+        <v>1342950</v>
+      </c>
+      <c r="F4">
+        <v>3634280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>356795</v>
+      </c>
+      <c r="C5">
+        <v>382480</v>
+      </c>
+      <c r="D5">
+        <v>185180</v>
+      </c>
+      <c r="E5">
+        <v>554328</v>
+      </c>
+      <c r="F5">
+        <v>739508</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6">
+        <v>14727</v>
+      </c>
+      <c r="C6">
+        <v>14710</v>
+      </c>
+      <c r="D6">
+        <v>8955</v>
+      </c>
+      <c r="E6">
+        <v>21060</v>
+      </c>
+      <c r="F6">
+        <v>30015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Hoja con gráfica de rectángulos
</commit_message>
<xml_diff>
--- a/08/GraficosII.xlsx
+++ b/08/GraficosII.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Iris" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,25 @@
     <sheet name="ColumnasApiladas" sheetId="5" r:id="rId5"/>
     <sheet name="Proporciones" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Proporciones!$A$33:$B$42</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Proporciones!$C$32</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Proporciones!$C$32</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Proporciones!$C$33:$C$42</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Proporciones!$A$33:$B$42</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Proporciones!$C$32</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Proporciones!$C$33:$C$42</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Proporciones!$A$73:$A$82</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Proporciones!$B$73:$B$82</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Proporciones!$C$33:$C$42</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Proporciones!$A$33:$B$42</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Proporciones!$C$32</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Proporciones!$C$33:$C$42</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Proporciones!$A$33:$B$42</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Proporciones!$C$32</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Proporciones!$C$33:$C$42</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Proporciones!$A$33:$B$42</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
@@ -30,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="33">
   <si>
     <t>Sepal.Length</t>
   </si>
@@ -126,6 +145,9 @@
   </si>
   <si>
     <t>Población</t>
+  </si>
+  <si>
+    <t>Sexo</t>
   </si>
 </sst>
 </file>
@@ -5311,11 +5333,236 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.12</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f>_xlchart.v1.14</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="sunburst" uniqueId="{22D7E61E-F0FE-4A7C-9F11-49B797FD7217}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:v>Población</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataLabels pos="ctr">
+            <cx:txPr>
+              <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES" sz="1400">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </cx:txPr>
+            <cx:visibility seriesName="0" categoryName="1" value="1"/>
+            <cx:separator>
+</cx:separator>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.15</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f>_xlchart.v1.16</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="treemap" uniqueId="{D40191E5-E9E9-428F-B697-0BC1F3FA5448}">
+          <cx:dataLabels pos="ctr">
+            <cx:txPr>
+              <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-ES">
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </a:endParaRPr>
+              </a:p>
+            </cx:txPr>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+            <cx:separator>, </cx:separator>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:parentLabelLayout val="overlapping"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="r" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f>_xlchart.v1.11</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="treemap" uniqueId="{026EBC8C-2EDA-4897-9223-2D2C5A4CB9D6}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:v>Población</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataLabels pos="inEnd">
+            <cx:visibility seriesName="0" categoryName="1" value="0"/>
+            <cx:separator>, </cx:separator>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:parentLabelLayout val="overlapping"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -5628,6 +5875,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6140,6 +6427,971 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="411">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1">
+          <a:lumMod val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr lIns="38100" tIns="19050" rIns="38100" bIns="19050">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+                <a:lumOff val="10000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+                <a:lumOff val="10000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="410">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1">
+          <a:lumMod val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="bg1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr lIns="38100" tIns="19050" rIns="38100" bIns="19050">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -9713,6 +10965,462 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="388">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="850" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr lIns="38100" tIns="19050" rIns="38100" bIns="19050">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="25000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+    <cs:bodyPr/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -9984,6 +11692,222 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Gráfico 2"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="247650" y="8001000"/>
+              <a:ext cx="6877050" cy="5267325"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Gráfico 3"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="161924" y="15735299"/>
+              <a:ext cx="8829675" cy="4286251"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Gráfico 4"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4095750" y="5514975"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -12836,7 +14760,7 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -13570,9 +15494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
@@ -13705,10 +15627,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -13833,6 +15755,207 @@
         <v>30015</v>
       </c>
     </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33">
+        <v>381985</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34">
+        <v>384409</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>404328</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36">
+        <v>413098</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37">
+        <v>1857046</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38">
+        <v>1777230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39">
+        <v>356795</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40">
+        <v>382480</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41">
+        <v>14727</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42">
+        <v>14710</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73">
+        <v>18701</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B74">
+        <v>4702</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75">
+        <v>3828</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B76">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B80">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B82">
+        <v>165</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Hoja con gráficas de distribución
</commit_message>
<xml_diff>
--- a/08/GraficosII.xlsx
+++ b/08/GraficosII.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Iris" sheetId="1" r:id="rId1"/>
@@ -18,25 +18,40 @@
     <sheet name="Valores acumulados" sheetId="4" r:id="rId4"/>
     <sheet name="ColumnasApiladas" sheetId="5" r:id="rId5"/>
     <sheet name="Proporciones" sheetId="6" r:id="rId6"/>
+    <sheet name="Distribución" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Proporciones!$A$33:$B$42</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Proporciones!$C$32</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Proporciones!$C$32</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Proporciones!$C$33:$C$42</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Proporciones!$A$33:$B$42</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Proporciones!$C$32</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Proporciones!$C$33:$C$42</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Proporciones!$A$73:$A$82</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Proporciones!$B$73:$B$82</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Proporciones!$B$73:$B$82</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Distribución!$A$40</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Distribución!$A$41:$A$190</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Distribución!$A$193:$A$200</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Distribución!$B$192</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Distribución!$B$193:$B$200</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Distribución!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Distribución!$B$1</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Distribución!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Distribución!$C$1</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Proporciones!$C$33:$C$42</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Distribución!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Distribución!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Distribución!$B$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Distribución!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Distribución!$C$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Distribución!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Distribución!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Distribución!$B$1</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Distribución!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Distribución!$C$1</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Proporciones!$A$33:$B$42</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Distribución!$C$2:$C$37</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Proporciones!$C$32</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Proporciones!$C$33:$C$42</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Proporciones!$A$33:$B$42</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">Proporciones!$C$32</definedName>
     <definedName name="_xlchart.v1.8" hidden="1">Proporciones!$C$33:$C$42</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Proporciones!$A$33:$B$42</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Proporciones!$A$73:$A$82</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -49,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="39">
   <si>
     <t>Sepal.Length</t>
   </si>
@@ -149,6 +164,24 @@
   <si>
     <t>Sexo</t>
   </si>
+  <si>
+    <t>Tipo de ataque</t>
+  </si>
+  <si>
+    <t>Fishing</t>
+  </si>
+  <si>
+    <t>Virus</t>
+  </si>
+  <si>
+    <t>Cookies</t>
+  </si>
+  <si>
+    <t>Gusano</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
 </sst>
 </file>
 
@@ -221,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -266,6 +299,9 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5338,10 +5374,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5351,7 +5387,7 @@
         <cx:series layoutId="sunburst" uniqueId="{22D7E61E-F0FE-4A7C-9F11-49B797FD7217}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:f>_xlchart.v1.7</cx:f>
               <cx:v>Población</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5393,10 +5429,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.16</cx:f>
+        <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5445,10 +5481,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5458,7 +5494,7 @@
         <cx:series layoutId="treemap" uniqueId="{026EBC8C-2EDA-4897-9223-2D2C5A4CB9D6}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Población</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5474,6 +5510,210 @@
       </cx:plotAreaRegion>
     </cx:plotArea>
     <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.26</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.28</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.26</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.30</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{06A8F964-2F9B-4C6D-ACD7-57AA8E910FF4}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.27</cx:f>
+              <cx:v>Rural</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{A91A7365-D57D-40AD-B2EB-0C6EF6AF838B}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.29</cx:f>
+              <cx:v>Urbana</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1.10000002"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling max="220000"/>
+        <cx:units unit="thousands"/>
+        <cx:majorGridlines/>
+        <cx:majorTickMarks type="in"/>
+        <cx:minorTickMarks type="in"/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.12</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Largo de pétalo</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES"/>
+            <a:t>Largo de pétalo</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{6412D0C7-A185-4A6F-89AB-8923F4A05303}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.11</cx:f>
+              <cx:v>Sepal.Length</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r">
+              <cx:binSize val="0.30000000000000004"/>
+            </cx:binning>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx6.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.13</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.15</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Tipos de ataque</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES"/>
+            <a:t>Tipos de ataque</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{C898AA8D-C54A-4A46-BDC9-3AB35E4C33F5}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:v>Cantidad</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:aggregation/>
+          </cx:layoutPr>
+          <cx:axisId val="1"/>
+        </cx:series>
+        <cx:series layoutId="paretoLine" ownerIdx="0" uniqueId="{9F58388D-49DC-4283-8D68-75E8287C097D}">
+          <cx:axisId val="2"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="2">
+        <cx:valScaling max="1" min="0"/>
+        <cx:units unit="percentage"/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
   </cx:chart>
 </cx:chartSpace>
 </file>
@@ -5556,6 +5796,126 @@
 </file>
 
 <file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -7396,6 +7756,1405 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="407">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+    <cs:bodyPr rot="0" vert="horz"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="367">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -11695,15 +13454,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>714375</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>733425</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -11733,7 +13492,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="247650" y="8001000"/>
+              <a:off x="714375" y="8105775"/>
               <a:ext cx="6877050" cy="5267325"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -11838,16 +13597,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -11877,8 +13636,229 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4095750" y="5514975"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="238124" y="20145374"/>
+              <a:ext cx="8753475" cy="4695825"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>104776</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Gráfico 4"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2390776" y="666750"/>
+              <a:ext cx="6238874" cy="4286250"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>633412</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="6" name="Gráfico 5"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1395412" y="7591424"/>
+              <a:ext cx="6719888" cy="4391026"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>414336</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="7" name="Gráfico 6"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1938336" y="36537899"/>
+              <a:ext cx="6300789" cy="4171951"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -12176,8 +14156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView topLeftCell="A122" workbookViewId="0">
-      <selection sqref="A1:D151"/>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection sqref="A1:A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -15311,7 +17291,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B21"/>
+      <selection activeCell="A2" sqref="A2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -15629,8 +17609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -15778,9 +17758,6 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>23</v>
-      </c>
       <c r="B34" t="s">
         <v>26</v>
       </c>
@@ -15800,9 +17777,6 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>27</v>
-      </c>
       <c r="B36" t="s">
         <v>26</v>
       </c>
@@ -15822,9 +17796,6 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>28</v>
-      </c>
       <c r="B38" t="s">
         <v>26</v>
       </c>
@@ -15844,9 +17815,6 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>29</v>
-      </c>
       <c r="B40" t="s">
         <v>26</v>
       </c>
@@ -15866,9 +17834,6 @@
       </c>
     </row>
     <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>30</v>
-      </c>
       <c r="B42" t="s">
         <v>26</v>
       </c>
@@ -15954,6 +17919,1390 @@
       </c>
       <c r="B82">
         <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C214"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="A207" sqref="A207"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="17">
+        <v>62031</v>
+      </c>
+      <c r="C2" s="17">
+        <v>46914</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="17">
+        <v>36519</v>
+      </c>
+      <c r="C3" s="17">
+        <v>30708</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="17">
+        <v>50600</v>
+      </c>
+      <c r="C4" s="17">
+        <v>10495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="17">
+        <v>35254</v>
+      </c>
+      <c r="C5" s="17">
+        <v>15081</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="17">
+        <v>19892</v>
+      </c>
+      <c r="C6" s="17">
+        <v>20008</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="17">
+        <v>23914</v>
+      </c>
+      <c r="C7" s="17">
+        <v>8878</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="17">
+        <v>12763</v>
+      </c>
+      <c r="C8" s="17">
+        <v>18011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="17">
+        <v>20050</v>
+      </c>
+      <c r="C9" s="17">
+        <v>9499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="17">
+        <v>18742</v>
+      </c>
+      <c r="C10" s="17">
+        <v>10141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="17">
+        <v>63543</v>
+      </c>
+      <c r="C11" s="17">
+        <v>212675</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="17">
+        <v>32439</v>
+      </c>
+      <c r="C12" s="17">
+        <v>135549</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="17">
+        <v>25126</v>
+      </c>
+      <c r="C13" s="17">
+        <v>72239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="17">
+        <v>10612</v>
+      </c>
+      <c r="C14" s="17">
+        <v>30952</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="17">
+        <v>3988</v>
+      </c>
+      <c r="C15" s="17">
+        <v>32589</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="17">
+        <v>7099</v>
+      </c>
+      <c r="C16" s="17">
+        <v>23758</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="17">
+        <v>6967</v>
+      </c>
+      <c r="C17" s="17">
+        <v>18262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="17">
+        <v>3071</v>
+      </c>
+      <c r="C18" s="17">
+        <v>20636</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="17">
+        <v>2334</v>
+      </c>
+      <c r="C19" s="17">
+        <v>12684</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="2">
+        <v>33375</v>
+      </c>
+      <c r="C20" s="2">
+        <v>113821</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="2">
+        <v>10411</v>
+      </c>
+      <c r="C21" s="2">
+        <v>71767</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="2">
+        <v>6335</v>
+      </c>
+      <c r="C22" s="2">
+        <v>52639</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="2">
+        <v>14495</v>
+      </c>
+      <c r="C23" s="2">
+        <v>44391</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="2">
+        <v>18969</v>
+      </c>
+      <c r="C24" s="2">
+        <v>38374</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="2">
+        <v>14166</v>
+      </c>
+      <c r="C25" s="2">
+        <v>36492</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2">
+        <v>8962</v>
+      </c>
+      <c r="C26" s="2">
+        <v>30672</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="2">
+        <v>13492</v>
+      </c>
+      <c r="C27" s="2">
+        <v>25248</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="2">
+        <v>9469</v>
+      </c>
+      <c r="C28" s="2">
+        <v>12933</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2863</v>
+      </c>
+      <c r="C29" s="2">
+        <v>15838</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2">
+        <v>3897</v>
+      </c>
+      <c r="C30" s="3">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3">
+        <v>509</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3">
+        <v>468</v>
+      </c>
+      <c r="C32" s="3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="3">
+        <v>348</v>
+      </c>
+      <c r="C33" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="3">
+        <v>100</v>
+      </c>
+      <c r="C34" s="3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="3">
+        <v>76</v>
+      </c>
+      <c r="C35" s="3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="3">
+        <v>149</v>
+      </c>
+      <c r="C36" s="3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="3">
+        <v>139</v>
+      </c>
+      <c r="C37" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
+        <v>33</v>
+      </c>
+      <c r="B192" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>34</v>
+      </c>
+      <c r="B193">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>34</v>
+      </c>
+      <c r="B194">
+        <f t="shared" ref="B194:B214" ca="1" si="0">RANDBETWEEN(1,100)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>35</v>
+      </c>
+      <c r="B195">
+        <f t="shared" ca="1" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>36</v>
+      </c>
+      <c r="B196">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
+        <v>35</v>
+      </c>
+      <c r="B197">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" t="s">
+        <v>36</v>
+      </c>
+      <c r="B198">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" t="s">
+        <v>37</v>
+      </c>
+      <c r="B199">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200" t="s">
+        <v>34</v>
+      </c>
+      <c r="B200">
+        <f t="shared" ca="1" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201" t="s">
+        <v>37</v>
+      </c>
+      <c r="B201">
+        <f t="shared" ca="1" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202" t="s">
+        <v>34</v>
+      </c>
+      <c r="B202">
+        <f t="shared" ca="1" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203" t="s">
+        <v>34</v>
+      </c>
+      <c r="B203">
+        <f t="shared" ca="1" si="0"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="A204" t="s">
+        <v>35</v>
+      </c>
+      <c r="B204">
+        <f t="shared" ca="1" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="A205" t="s">
+        <v>36</v>
+      </c>
+      <c r="B205">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206" t="s">
+        <v>35</v>
+      </c>
+      <c r="B206">
+        <f t="shared" ca="1" si="0"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="A207" t="s">
+        <v>36</v>
+      </c>
+      <c r="B207">
+        <f t="shared" ca="1" si="0"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" t="s">
+        <v>37</v>
+      </c>
+      <c r="B208">
+        <f t="shared" ca="1" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" t="s">
+        <v>34</v>
+      </c>
+      <c r="B209">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" t="s">
+        <v>34</v>
+      </c>
+      <c r="B210">
+        <f t="shared" ca="1" si="0"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" t="s">
+        <v>34</v>
+      </c>
+      <c r="B211">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" t="s">
+        <v>35</v>
+      </c>
+      <c r="B212">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" t="s">
+        <v>36</v>
+      </c>
+      <c r="B213">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" t="s">
+        <v>35</v>
+      </c>
+      <c r="B214">
+        <f t="shared" ca="1" si="0"/>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hoja con la gráfica de dispersión
</commit_message>
<xml_diff>
--- a/08/GraficosII.xlsx
+++ b/08/GraficosII.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400"/>
   </bookViews>
   <sheets>
-    <sheet name="Iris" sheetId="1" r:id="rId1"/>
+    <sheet name="Dispersión" sheetId="1" r:id="rId1"/>
     <sheet name="Datos discretos" sheetId="2" r:id="rId2"/>
     <sheet name="Valores continuos" sheetId="3" r:id="rId3"/>
     <sheet name="Valores acumulados" sheetId="4" r:id="rId4"/>
@@ -26,26 +26,34 @@
     <definedName name="_xlchart.v1.10" hidden="1">Proporciones!$B$73:$B$82</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">Distribución!$A$40</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">Distribución!$A$41:$A$190</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Distribución!$A$193:$A$200</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Distribución!$B$192</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Distribución!$B$193:$B$200</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Distribución!$A$2:$A$37</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Distribución!$B$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Distribución!$B$2:$B$37</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Distribución!$C$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Distribución!$B$40</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Distribución!$B$41:$B$190</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Distribución!$C$40</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Distribución!$C$41:$C$190</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Distribución!$D$40</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Distribución!$D$41:$D$190</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Distribución!$A$40</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Proporciones!$C$33:$C$42</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Distribución!$C$2:$C$37</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Distribución!$A$2:$A$37</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Distribución!$B$1</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Distribución!$B$2:$B$37</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Distribución!$C$1</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Distribución!$C$2:$C$37</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Distribución!$A$2:$A$37</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Distribución!$B$1</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Distribución!$B$2:$B$37</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Distribución!$C$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Distribución!$A$41:$A$190</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Distribución!$A$193:$A$200</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Distribución!$B$192</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Distribución!$B$193:$B$200</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Distribución!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Distribución!$B$1</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Distribución!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Distribución!$C$1</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Distribución!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Distribución!$A$2:$A$37</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Proporciones!$A$33:$B$42</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Distribución!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Distribución!$B$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Distribución!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Distribución!$C$1</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Distribución!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Distribución!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Distribución!$B$1</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Distribución!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Distribución!$C$1</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Distribución!$C$2:$C$37</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Proporciones!$C$32</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Proporciones!$C$33:$C$42</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">Proporciones!$A$33:$B$42</definedName>
@@ -64,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="39">
   <si>
     <t>Sepal.Length</t>
   </si>
@@ -370,7 +378,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -402,7 +410,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -431,30 +439,66 @@
             <c:v>setosa</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="4"/>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent6"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Iris!$C$2:$C$51</c:f>
+              <c:f>Dispersión!$C$2:$C$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -613,7 +657,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Iris!$D$2:$D$51</c:f>
+              <c:f>Dispersión!$D$2:$D$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -788,26 +832,62 @@
               <a:noFill/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="4"/>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent5">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent5">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent5"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Iris!$C$52:$C$101</c:f>
+              <c:f>Dispersión!$C$52:$C$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -966,7 +1046,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Iris!$D$52:$D$101</c:f>
+              <c:f>Dispersión!$D$52:$D$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -1141,26 +1221,62 @@
               <a:noFill/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="4"/>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent4"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Iris!$C$102:$C$151</c:f>
+              <c:f>Dispersión!$C$102:$C$151</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -1319,7 +1435,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Iris!$D$102:$D$151</c:f>
+              <c:f>Dispersión!$D$102:$D$151</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
@@ -1524,7 +1640,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1556,7 +1672,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1578,14 +1694,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1642,7 +1752,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1674,7 +1784,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1696,14 +1806,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1740,7 +1844,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5519,18 +5623,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.26</cx:f>
+        <cx:f>_xlchart.v1.34</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.28</cx:f>
+        <cx:f>_xlchart.v1.36</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.26</cx:f>
+        <cx:f>_xlchart.v1.34</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.30</cx:f>
+        <cx:f>_xlchart.v1.38</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5541,7 +5645,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{06A8F964-2F9B-4C6D-ACD7-57AA8E910FF4}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.27</cx:f>
+              <cx:f>_xlchart.v1.35</cx:f>
               <cx:v>Rural</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5554,7 +5658,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{A91A7365-D57D-40AD-B2EB-0C6EF6AF838B}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.29</cx:f>
+              <cx:f>_xlchart.v1.37</cx:f>
               <cx:v>Urbana</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5588,7 +5692,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.20</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5618,7 +5722,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{6412D0C7-A185-4A6F-89AB-8923F4A05303}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.11</cx:f>
+              <cx:f>_xlchart.v1.19</cx:f>
               <cx:v>Sepal.Length</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5652,10 +5756,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5685,7 +5789,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{C898AA8D-C54A-4A46-BDC9-3AB35E4C33F5}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:f>_xlchart.v1.22</cx:f>
               <cx:v>Cantidad</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5711,6 +5815,120 @@
       <cx:axis id="2">
         <cx:valScaling max="1" min="0"/>
         <cx:units unit="percentage"/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx7.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.12</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.14</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.16</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.18</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Longitud y ancho de pétalo y sépalo en Iris</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES"/>
+            <a:t>Longitud y ancho de pétalo y sépalo en Iris</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{69B1952C-81DB-4BCD-A143-96858D6E7D05}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.11</cx:f>
+              <cx:v>Sepal.Length</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{20CD4C99-5325-424F-B86B-210292E05602}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:v>Sepal.Width</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{F03F70D5-09C7-4A72-9DC7-A75436780008}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.15</cx:f>
+              <cx:v>Petal.Length</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{F114C8F3-BDCD-43A3-B2B4-09F48BE81A2F}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.17</cx:f>
+              <cx:v>Petal.Width</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0" hidden="1">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling max="8" min="0"/>
+        <cx:majorGridlines/>
         <cx:tickLabels/>
       </cx:axis>
     </cx:plotArea>
@@ -5916,6 +6134,46 @@
 </file>
 
 <file path=xl/charts/colors14.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6276,7 +6534,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -6287,7 +6545,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -6300,11 +6558,11 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6317,7 +6575,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx2"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -6333,7 +6591,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -6377,20 +6635,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -6399,13 +6657,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -6417,30 +6675,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -6480,23 +6739,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -6543,14 +6801,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -6601,8 +6853,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6640,20 +6892,20 @@
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -6666,6 +6918,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -6697,7 +6960,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -6706,14 +6969,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -6734,20 +6996,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -6761,17 +7022,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6779,14 +7029,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -9143,6 +9387,492 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:bodyPr rot="0" vert="horz"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -13746,16 +14476,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>633412</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>490537</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -13785,7 +14515,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1395412" y="7591424"/>
+              <a:off x="2776537" y="8086724"/>
               <a:ext cx="6719888" cy="4391026"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -13859,6 +14589,78 @@
             <a:xfrm>
               <a:off x="1938336" y="36537899"/>
               <a:ext cx="6300789" cy="4171951"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="8" name="Gráfico 7"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3405187" y="5133975"/>
+              <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -14156,11 +14958,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection sqref="A1:A151"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -17929,10 +18737,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:D214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="A207" sqref="A207"/>
+    <sheetView topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -18289,7 +19097,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -18300,7 +19108,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -18311,7 +19119,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -18322,7 +19130,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -18333,7 +19141,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -18344,762 +19152,2121 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="B41">
+        <v>3.5</v>
+      </c>
+      <c r="C41">
+        <v>1.4</v>
+      </c>
+      <c r="D41">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>1.4</v>
+      </c>
+      <c r="D42">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="B43">
+        <v>3.2</v>
+      </c>
+      <c r="C43">
+        <v>1.3</v>
+      </c>
+      <c r="D43">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="B44">
+        <v>3.1</v>
+      </c>
+      <c r="C44">
+        <v>1.5</v>
+      </c>
+      <c r="D44">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="B45">
+        <v>3.6</v>
+      </c>
+      <c r="C45">
+        <v>1.4</v>
+      </c>
+      <c r="D45">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="B46">
+        <v>3.9</v>
+      </c>
+      <c r="C46">
+        <v>1.7</v>
+      </c>
+      <c r="D46">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="B47">
+        <v>3.4</v>
+      </c>
+      <c r="C47">
+        <v>1.4</v>
+      </c>
+      <c r="D47">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48">
+        <v>3.4</v>
+      </c>
+      <c r="C48">
+        <v>1.5</v>
+      </c>
+      <c r="D48">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49">
+        <v>2.9</v>
+      </c>
+      <c r="C49">
+        <v>1.4</v>
+      </c>
+      <c r="D49">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50">
+        <v>3.1</v>
+      </c>
+      <c r="C50">
+        <v>1.5</v>
+      </c>
+      <c r="D50">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51">
+        <v>3.7</v>
+      </c>
+      <c r="C51">
+        <v>1.5</v>
+      </c>
+      <c r="D51">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52">
+        <v>3.4</v>
+      </c>
+      <c r="C52">
+        <v>1.6</v>
+      </c>
+      <c r="D52">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>1.4</v>
+      </c>
+      <c r="D53">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D54">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>1.2</v>
+      </c>
+      <c r="D55">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C56">
+        <v>1.5</v>
+      </c>
+      <c r="D56">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57">
+        <v>3.9</v>
+      </c>
+      <c r="C57">
+        <v>1.3</v>
+      </c>
+      <c r="D57">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58">
+        <v>3.5</v>
+      </c>
+      <c r="C58">
+        <v>1.4</v>
+      </c>
+      <c r="D58">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59">
+        <v>3.8</v>
+      </c>
+      <c r="C59">
+        <v>1.7</v>
+      </c>
+      <c r="D59">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="B60">
+        <v>3.8</v>
+      </c>
+      <c r="C60">
+        <v>1.5</v>
+      </c>
+      <c r="D60">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="B61">
+        <v>3.4</v>
+      </c>
+      <c r="C61">
+        <v>1.7</v>
+      </c>
+      <c r="D61">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="B62">
+        <v>3.7</v>
+      </c>
+      <c r="C62">
+        <v>1.5</v>
+      </c>
+      <c r="D62">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="B63">
+        <v>3.6</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64">
+        <v>3.3</v>
+      </c>
+      <c r="C64">
+        <v>1.7</v>
+      </c>
+      <c r="D64">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65">
+        <v>3.4</v>
+      </c>
+      <c r="C65">
+        <v>1.9</v>
+      </c>
+      <c r="D65">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66">
+        <v>1.6</v>
+      </c>
+      <c r="D66">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>5</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67">
+        <v>3.4</v>
+      </c>
+      <c r="C67">
+        <v>1.6</v>
+      </c>
+      <c r="D67">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68">
+        <v>3.5</v>
+      </c>
+      <c r="C68">
+        <v>1.5</v>
+      </c>
+      <c r="D68">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69">
+        <v>3.4</v>
+      </c>
+      <c r="C69">
+        <v>1.4</v>
+      </c>
+      <c r="D69">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>4.7</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70">
+        <v>3.2</v>
+      </c>
+      <c r="C70">
+        <v>1.6</v>
+      </c>
+      <c r="D70">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="B71">
+        <v>3.1</v>
+      </c>
+      <c r="C71">
+        <v>1.6</v>
+      </c>
+      <c r="D71">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72">
+        <v>3.4</v>
+      </c>
+      <c r="C72">
+        <v>1.5</v>
+      </c>
+      <c r="D72">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C73">
+        <v>1.5</v>
+      </c>
+      <c r="D73">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74">
+        <v>4.2</v>
+      </c>
+      <c r="C74">
+        <v>1.4</v>
+      </c>
+      <c r="D74">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75">
+        <v>3.1</v>
+      </c>
+      <c r="C75">
+        <v>1.5</v>
+      </c>
+      <c r="D75">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
+      <c r="B76">
+        <v>3.2</v>
+      </c>
+      <c r="C76">
+        <v>1.2</v>
+      </c>
+      <c r="D76">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
+      <c r="B77">
+        <v>3.5</v>
+      </c>
+      <c r="C77">
+        <v>1.3</v>
+      </c>
+      <c r="D77">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="B78">
+        <v>3.6</v>
+      </c>
+      <c r="C78">
+        <v>1.4</v>
+      </c>
+      <c r="D78">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="B79">
+        <v>3</v>
+      </c>
+      <c r="C79">
+        <v>1.3</v>
+      </c>
+      <c r="D79">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80">
+        <v>3.4</v>
+      </c>
+      <c r="C80">
+        <v>1.5</v>
+      </c>
+      <c r="D80">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81">
+        <v>3.5</v>
+      </c>
+      <c r="C81">
+        <v>1.3</v>
+      </c>
+      <c r="D81">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
+      <c r="B82">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C82">
+        <v>1.3</v>
+      </c>
+      <c r="D82">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="B83">
+        <v>3.2</v>
+      </c>
+      <c r="C83">
+        <v>1.3</v>
+      </c>
+      <c r="D83">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
+      <c r="B84">
+        <v>3.5</v>
+      </c>
+      <c r="C84">
+        <v>1.6</v>
+      </c>
+      <c r="D84">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="B85">
+        <v>3.8</v>
+      </c>
+      <c r="C85">
+        <v>1.9</v>
+      </c>
+      <c r="D85">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="87" spans="1:1">
+      <c r="B86">
+        <v>3</v>
+      </c>
+      <c r="C86">
+        <v>1.4</v>
+      </c>
+      <c r="D86">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="88" spans="1:1">
+      <c r="B87">
+        <v>3.8</v>
+      </c>
+      <c r="C87">
+        <v>1.6</v>
+      </c>
+      <c r="D87">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
+      <c r="B88">
+        <v>3.2</v>
+      </c>
+      <c r="C88">
+        <v>1.4</v>
+      </c>
+      <c r="D88">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="90" spans="1:1">
+      <c r="B89">
+        <v>3.7</v>
+      </c>
+      <c r="C89">
+        <v>1.5</v>
+      </c>
+      <c r="D89">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" spans="1:1">
+      <c r="B90">
+        <v>3.3</v>
+      </c>
+      <c r="C90">
+        <v>1.4</v>
+      </c>
+      <c r="D90">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91">
         <v>7</v>
       </c>
-    </row>
-    <row r="92" spans="1:1">
+      <c r="B91">
+        <v>3.2</v>
+      </c>
+      <c r="C91">
+        <v>4.7</v>
+      </c>
+      <c r="D91">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="93" spans="1:1">
+      <c r="B92">
+        <v>3.2</v>
+      </c>
+      <c r="C92">
+        <v>4.5</v>
+      </c>
+      <c r="D92">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="94" spans="1:1">
+      <c r="B93">
+        <v>3.1</v>
+      </c>
+      <c r="C93">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D93">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="95" spans="1:1">
+      <c r="B94">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C94">
+        <v>4</v>
+      </c>
+      <c r="D94">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
+      <c r="B95">
+        <v>2.8</v>
+      </c>
+      <c r="C95">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D95">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="B96">
+        <v>2.8</v>
+      </c>
+      <c r="C96">
+        <v>4.5</v>
+      </c>
+      <c r="D96">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="B97">
+        <v>3.3</v>
+      </c>
+      <c r="C97">
+        <v>4.7</v>
+      </c>
+      <c r="D97">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="99" spans="1:1">
+      <c r="B98">
+        <v>2.4</v>
+      </c>
+      <c r="C98">
+        <v>3.3</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99">
         <v>6.6</v>
       </c>
-    </row>
-    <row r="100" spans="1:1">
+      <c r="B99">
+        <v>2.9</v>
+      </c>
+      <c r="C99">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D99">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="101" spans="1:1">
+      <c r="B100">
+        <v>2.7</v>
+      </c>
+      <c r="C100">
+        <v>3.9</v>
+      </c>
+      <c r="D100">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="B101">
+        <v>2</v>
+      </c>
+      <c r="C101">
+        <v>3.5</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="103" spans="1:1">
+      <c r="B102">
+        <v>3</v>
+      </c>
+      <c r="C102">
+        <v>4.2</v>
+      </c>
+      <c r="D102">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103">
         <v>6</v>
       </c>
-    </row>
-    <row r="104" spans="1:1">
+      <c r="B103">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C103">
+        <v>4</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="105" spans="1:1">
+      <c r="B104">
+        <v>2.9</v>
+      </c>
+      <c r="C104">
+        <v>4.7</v>
+      </c>
+      <c r="D104">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="106" spans="1:1">
+      <c r="B105">
+        <v>2.9</v>
+      </c>
+      <c r="C105">
+        <v>3.6</v>
+      </c>
+      <c r="D105">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="107" spans="1:1">
+      <c r="B106">
+        <v>3.1</v>
+      </c>
+      <c r="C106">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D106">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="108" spans="1:1">
+      <c r="B107">
+        <v>3</v>
+      </c>
+      <c r="C107">
+        <v>4.5</v>
+      </c>
+      <c r="D107">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="109" spans="1:1">
+      <c r="B108">
+        <v>2.7</v>
+      </c>
+      <c r="C108">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109">
         <v>6.2</v>
       </c>
-    </row>
-    <row r="110" spans="1:1">
+      <c r="B109">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C109">
+        <v>4.5</v>
+      </c>
+      <c r="D109">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="111" spans="1:1">
+      <c r="B110">
+        <v>2.5</v>
+      </c>
+      <c r="C110">
+        <v>3.9</v>
+      </c>
+      <c r="D110">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="112" spans="1:1">
+      <c r="B111">
+        <v>3.2</v>
+      </c>
+      <c r="C111">
+        <v>4.8</v>
+      </c>
+      <c r="D111">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="B112">
+        <v>2.8</v>
+      </c>
+      <c r="C112">
+        <v>4</v>
+      </c>
+      <c r="D112">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="B113">
+        <v>2.5</v>
+      </c>
+      <c r="C113">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D113">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="115" spans="1:1">
+      <c r="B114">
+        <v>2.8</v>
+      </c>
+      <c r="C114">
+        <v>4.7</v>
+      </c>
+      <c r="D114">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="116" spans="1:1">
+      <c r="B115">
+        <v>2.9</v>
+      </c>
+      <c r="C115">
+        <v>4.3</v>
+      </c>
+      <c r="D115">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116">
         <v>6.6</v>
       </c>
-    </row>
-    <row r="117" spans="1:1">
+      <c r="B116">
+        <v>3</v>
+      </c>
+      <c r="C116">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D116">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="118" spans="1:1">
+      <c r="B117">
+        <v>2.8</v>
+      </c>
+      <c r="C117">
+        <v>4.8</v>
+      </c>
+      <c r="D117">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="119" spans="1:1">
+      <c r="B118">
+        <v>3</v>
+      </c>
+      <c r="C118">
+        <v>5</v>
+      </c>
+      <c r="D118">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119">
         <v>6</v>
       </c>
-    </row>
-    <row r="120" spans="1:1">
+      <c r="B119">
+        <v>2.9</v>
+      </c>
+      <c r="C119">
+        <v>4.5</v>
+      </c>
+      <c r="D119">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="121" spans="1:1">
+      <c r="B120">
+        <v>2.6</v>
+      </c>
+      <c r="C120">
+        <v>3.5</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="122" spans="1:1">
+      <c r="B121">
+        <v>2.4</v>
+      </c>
+      <c r="C121">
+        <v>3.8</v>
+      </c>
+      <c r="D121">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="123" spans="1:1">
+      <c r="B122">
+        <v>2.4</v>
+      </c>
+      <c r="C122">
+        <v>3.7</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="124" spans="1:1">
+      <c r="B123">
+        <v>2.7</v>
+      </c>
+      <c r="C123">
+        <v>3.9</v>
+      </c>
+      <c r="D123">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124">
         <v>6</v>
       </c>
-    </row>
-    <row r="125" spans="1:1">
+      <c r="B124">
+        <v>2.7</v>
+      </c>
+      <c r="C124">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D124">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="126" spans="1:1">
+      <c r="B125">
+        <v>3</v>
+      </c>
+      <c r="C125">
+        <v>4.5</v>
+      </c>
+      <c r="D125">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126">
         <v>6</v>
       </c>
-    </row>
-    <row r="127" spans="1:1">
+      <c r="B126">
+        <v>3.4</v>
+      </c>
+      <c r="C126">
+        <v>4.5</v>
+      </c>
+      <c r="D126">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="128" spans="1:1">
+      <c r="B127">
+        <v>3.1</v>
+      </c>
+      <c r="C127">
+        <v>4.7</v>
+      </c>
+      <c r="D127">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="129" spans="1:1">
+      <c r="B128">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C128">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D128">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="130" spans="1:1">
+      <c r="B129">
+        <v>3</v>
+      </c>
+      <c r="C129">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D129">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="131" spans="1:1">
+      <c r="B130">
+        <v>2.5</v>
+      </c>
+      <c r="C130">
+        <v>4</v>
+      </c>
+      <c r="D130">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="132" spans="1:1">
+      <c r="B131">
+        <v>2.6</v>
+      </c>
+      <c r="C131">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D131">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="133" spans="1:1">
+      <c r="B132">
+        <v>3</v>
+      </c>
+      <c r="C132">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D132">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="134" spans="1:1">
+      <c r="B133">
+        <v>2.6</v>
+      </c>
+      <c r="C133">
+        <v>4</v>
+      </c>
+      <c r="D133">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134">
         <v>5</v>
       </c>
-    </row>
-    <row r="135" spans="1:1">
+      <c r="B134">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C134">
+        <v>3.3</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="136" spans="1:1">
+      <c r="B135">
+        <v>2.7</v>
+      </c>
+      <c r="C135">
+        <v>4.2</v>
+      </c>
+      <c r="D135">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="137" spans="1:1">
+      <c r="B136">
+        <v>3</v>
+      </c>
+      <c r="C136">
+        <v>4.2</v>
+      </c>
+      <c r="D136">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="138" spans="1:1">
+      <c r="B137">
+        <v>2.9</v>
+      </c>
+      <c r="C137">
+        <v>4.2</v>
+      </c>
+      <c r="D137">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138">
         <v>6.2</v>
       </c>
-    </row>
-    <row r="139" spans="1:1">
+      <c r="B138">
+        <v>2.9</v>
+      </c>
+      <c r="C138">
+        <v>4.3</v>
+      </c>
+      <c r="D138">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="140" spans="1:1">
+      <c r="B139">
+        <v>2.5</v>
+      </c>
+      <c r="C139">
+        <v>3</v>
+      </c>
+      <c r="D139">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="141" spans="1:1">
+      <c r="B140">
+        <v>2.8</v>
+      </c>
+      <c r="C140">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D140">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="142" spans="1:1">
+      <c r="B141">
+        <v>3.3</v>
+      </c>
+      <c r="C141">
+        <v>6</v>
+      </c>
+      <c r="D141">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="143" spans="1:1">
+      <c r="B142">
+        <v>2.7</v>
+      </c>
+      <c r="C142">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D142">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="144" spans="1:1">
+      <c r="B143">
+        <v>3</v>
+      </c>
+      <c r="C143">
+        <v>5.9</v>
+      </c>
+      <c r="D143">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="145" spans="1:1">
+      <c r="B144">
+        <v>2.9</v>
+      </c>
+      <c r="C144">
+        <v>5.6</v>
+      </c>
+      <c r="D144">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="146" spans="1:1">
+      <c r="B145">
+        <v>3</v>
+      </c>
+      <c r="C145">
+        <v>5.8</v>
+      </c>
+      <c r="D145">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146">
         <v>7.6</v>
       </c>
-    </row>
-    <row r="147" spans="1:1">
+      <c r="B146">
+        <v>3</v>
+      </c>
+      <c r="C146">
+        <v>6.6</v>
+      </c>
+      <c r="D146">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="148" spans="1:1">
+      <c r="B147">
+        <v>2.5</v>
+      </c>
+      <c r="C147">
+        <v>4.5</v>
+      </c>
+      <c r="D147">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="149" spans="1:1">
+      <c r="B148">
+        <v>2.9</v>
+      </c>
+      <c r="C148">
+        <v>6.3</v>
+      </c>
+      <c r="D148">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="150" spans="1:1">
+      <c r="B149">
+        <v>2.5</v>
+      </c>
+      <c r="C149">
+        <v>5.8</v>
+      </c>
+      <c r="D149">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="151" spans="1:1">
+      <c r="B150">
+        <v>3.6</v>
+      </c>
+      <c r="C150">
+        <v>6.1</v>
+      </c>
+      <c r="D150">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="152" spans="1:1">
+      <c r="B151">
+        <v>3.2</v>
+      </c>
+      <c r="C151">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="153" spans="1:1">
+      <c r="B152">
+        <v>2.7</v>
+      </c>
+      <c r="C152">
+        <v>5.3</v>
+      </c>
+      <c r="D152">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="154" spans="1:1">
+      <c r="B153">
+        <v>3</v>
+      </c>
+      <c r="C153">
+        <v>5.5</v>
+      </c>
+      <c r="D153">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="155" spans="1:1">
+      <c r="B154">
+        <v>2.5</v>
+      </c>
+      <c r="C154">
+        <v>5</v>
+      </c>
+      <c r="D154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="156" spans="1:1">
+      <c r="B155">
+        <v>2.8</v>
+      </c>
+      <c r="C155">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D155">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="157" spans="1:1">
+      <c r="B156">
+        <v>3.2</v>
+      </c>
+      <c r="C156">
+        <v>5.3</v>
+      </c>
+      <c r="D156">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="158" spans="1:1">
+      <c r="B157">
+        <v>3</v>
+      </c>
+      <c r="C157">
+        <v>5.5</v>
+      </c>
+      <c r="D157">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="159" spans="1:1">
+      <c r="B158">
+        <v>3.8</v>
+      </c>
+      <c r="C158">
+        <v>6.7</v>
+      </c>
+      <c r="D158">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
       <c r="A159">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="160" spans="1:1">
+      <c r="B159">
+        <v>2.6</v>
+      </c>
+      <c r="C159">
+        <v>6.9</v>
+      </c>
+      <c r="D159">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
       <c r="A160">
         <v>6</v>
       </c>
-    </row>
-    <row r="161" spans="1:1">
+      <c r="B160">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C160">
+        <v>5</v>
+      </c>
+      <c r="D160">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
       <c r="A161">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="162" spans="1:1">
+      <c r="B161">
+        <v>3.2</v>
+      </c>
+      <c r="C161">
+        <v>5.7</v>
+      </c>
+      <c r="D161">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="163" spans="1:1">
+      <c r="B162">
+        <v>2.8</v>
+      </c>
+      <c r="C162">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D162">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="164" spans="1:1">
+      <c r="B163">
+        <v>2.8</v>
+      </c>
+      <c r="C163">
+        <v>6.7</v>
+      </c>
+      <c r="D163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="165" spans="1:1">
+      <c r="B164">
+        <v>2.7</v>
+      </c>
+      <c r="C164">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D164">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="166" spans="1:1">
+      <c r="B165">
+        <v>3.3</v>
+      </c>
+      <c r="C165">
+        <v>5.7</v>
+      </c>
+      <c r="D165">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="167" spans="1:1">
+      <c r="B166">
+        <v>3.2</v>
+      </c>
+      <c r="C166">
+        <v>6</v>
+      </c>
+      <c r="D166">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
       <c r="A167">
         <v>6.2</v>
       </c>
-    </row>
-    <row r="168" spans="1:1">
+      <c r="B167">
+        <v>2.8</v>
+      </c>
+      <c r="C167">
+        <v>4.8</v>
+      </c>
+      <c r="D167">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
       <c r="A168">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="169" spans="1:1">
+      <c r="B168">
+        <v>3</v>
+      </c>
+      <c r="C168">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D168">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
       <c r="A169">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="170" spans="1:1">
+      <c r="B169">
+        <v>2.8</v>
+      </c>
+      <c r="C169">
+        <v>5.6</v>
+      </c>
+      <c r="D169">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
       <c r="A170">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="171" spans="1:1">
+      <c r="B170">
+        <v>3</v>
+      </c>
+      <c r="C170">
+        <v>5.8</v>
+      </c>
+      <c r="D170">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
       <c r="A171">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="172" spans="1:1">
+      <c r="B171">
+        <v>2.8</v>
+      </c>
+      <c r="C171">
+        <v>6.1</v>
+      </c>
+      <c r="D171">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
       <c r="A172">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="173" spans="1:1">
+      <c r="B172">
+        <v>3.8</v>
+      </c>
+      <c r="C172">
+        <v>6.4</v>
+      </c>
+      <c r="D172">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="174" spans="1:1">
+      <c r="B173">
+        <v>2.8</v>
+      </c>
+      <c r="C173">
+        <v>5.6</v>
+      </c>
+      <c r="D173">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
       <c r="A174">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="175" spans="1:1">
+      <c r="B174">
+        <v>2.8</v>
+      </c>
+      <c r="C174">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D174">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
       <c r="A175">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="176" spans="1:1">
+      <c r="B175">
+        <v>2.6</v>
+      </c>
+      <c r="C175">
+        <v>5.6</v>
+      </c>
+      <c r="D175">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
       <c r="A176">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="177" spans="1:2">
+      <c r="B176">
+        <v>3</v>
+      </c>
+      <c r="C176">
+        <v>6.1</v>
+      </c>
+      <c r="D176">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
       <c r="A177">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="178" spans="1:2">
+      <c r="B177">
+        <v>3.4</v>
+      </c>
+      <c r="C177">
+        <v>5.6</v>
+      </c>
+      <c r="D177">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
       <c r="A178">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="179" spans="1:2">
+      <c r="B178">
+        <v>3.1</v>
+      </c>
+      <c r="C178">
+        <v>5.5</v>
+      </c>
+      <c r="D178">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
       <c r="A179">
         <v>6</v>
       </c>
-    </row>
-    <row r="180" spans="1:2">
+      <c r="B179">
+        <v>3</v>
+      </c>
+      <c r="C179">
+        <v>4.8</v>
+      </c>
+      <c r="D179">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
       <c r="A180">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="181" spans="1:2">
+      <c r="B180">
+        <v>3.1</v>
+      </c>
+      <c r="C180">
+        <v>5.4</v>
+      </c>
+      <c r="D180">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
       <c r="A181">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="182" spans="1:2">
+      <c r="B181">
+        <v>3.1</v>
+      </c>
+      <c r="C181">
+        <v>5.6</v>
+      </c>
+      <c r="D181">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
       <c r="A182">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="183" spans="1:2">
+      <c r="B182">
+        <v>3.1</v>
+      </c>
+      <c r="C182">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D182">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
       <c r="A183">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="184" spans="1:2">
+      <c r="B183">
+        <v>2.7</v>
+      </c>
+      <c r="C183">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D183">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
       <c r="A184">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="185" spans="1:2">
+      <c r="B184">
+        <v>3.2</v>
+      </c>
+      <c r="C184">
+        <v>5.9</v>
+      </c>
+      <c r="D184">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
       <c r="A185">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="186" spans="1:2">
+      <c r="B185">
+        <v>3.3</v>
+      </c>
+      <c r="C185">
+        <v>5.7</v>
+      </c>
+      <c r="D185">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
       <c r="A186">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="187" spans="1:2">
+      <c r="B186">
+        <v>3</v>
+      </c>
+      <c r="C186">
+        <v>5.2</v>
+      </c>
+      <c r="D186">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
       <c r="A187">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="188" spans="1:2">
+      <c r="B187">
+        <v>2.5</v>
+      </c>
+      <c r="C187">
+        <v>5</v>
+      </c>
+      <c r="D187">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
       <c r="A188">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="189" spans="1:2">
+      <c r="B188">
+        <v>3</v>
+      </c>
+      <c r="C188">
+        <v>5.2</v>
+      </c>
+      <c r="D188">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
       <c r="A189">
         <v>6.2</v>
       </c>
-    </row>
-    <row r="190" spans="1:2">
+      <c r="B189">
+        <v>3.4</v>
+      </c>
+      <c r="C189">
+        <v>5.4</v>
+      </c>
+      <c r="D189">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
       <c r="A190">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="192" spans="1:2">
+      <c r="B190">
+        <v>3</v>
+      </c>
+      <c r="C190">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D190">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
       <c r="A192" t="s">
         <v>33</v>
       </c>
@@ -19113,7 +21280,7 @@
       </c>
       <c r="B193">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -19122,7 +21289,7 @@
       </c>
       <c r="B194">
         <f t="shared" ref="B194:B214" ca="1" si="0">RANDBETWEEN(1,100)</f>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -19131,7 +21298,7 @@
       </c>
       <c r="B195">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -19140,7 +21307,7 @@
       </c>
       <c r="B196">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -19149,7 +21316,7 @@
       </c>
       <c r="B197">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -19158,7 +21325,7 @@
       </c>
       <c r="B198">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>59</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -19167,7 +21334,7 @@
       </c>
       <c r="B199">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>96</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -19176,7 +21343,7 @@
       </c>
       <c r="B200">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -19185,7 +21352,7 @@
       </c>
       <c r="B201">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -19194,7 +21361,7 @@
       </c>
       <c r="B202">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -19203,7 +21370,7 @@
       </c>
       <c r="B203">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>89</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -19212,7 +21379,7 @@
       </c>
       <c r="B204">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -19221,7 +21388,7 @@
       </c>
       <c r="B205">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -19230,7 +21397,7 @@
       </c>
       <c r="B206">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -19239,7 +21406,7 @@
       </c>
       <c r="B207">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>25</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -19248,7 +21415,7 @@
       </c>
       <c r="B208">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -19257,7 +21424,7 @@
       </c>
       <c r="B209">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>81</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -19266,7 +21433,7 @@
       </c>
       <c r="B210">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -19275,7 +21442,7 @@
       </c>
       <c r="B211">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>92</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -19284,7 +21451,7 @@
       </c>
       <c r="B212">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -19293,7 +21460,7 @@
       </c>
       <c r="B213">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>82</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -19302,7 +21469,7 @@
       </c>
       <c r="B214">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hoja con gráfica de cascada
</commit_message>
<xml_diff>
--- a/08/GraficosII.xlsx
+++ b/08/GraficosII.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Dispersión" sheetId="1" r:id="rId1"/>
@@ -19,47 +19,37 @@
     <sheet name="ColumnasApiladas" sheetId="5" r:id="rId5"/>
     <sheet name="Proporciones" sheetId="6" r:id="rId6"/>
     <sheet name="Distribución" sheetId="7" r:id="rId7"/>
+    <sheet name="Hoja3" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Proporciones!$A$33:$B$42</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Proporciones!$C$32</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Proporciones!$B$73:$B$82</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Distribución!$A$40</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Distribución!$A$41:$A$190</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Distribución!$B$40</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Distribución!$B$41:$B$190</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Distribución!$C$40</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Distribución!$C$41:$C$190</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Distribución!$D$40</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Distribución!$D$41:$D$190</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Distribución!$A$40</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Distribución!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Distribución!$C$1</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Distribución!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Distribución!$A$193:$A$200</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Distribución!$B$192</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Distribución!$B$193:$B$200</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Distribución!$A$40</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Distribución!$A$41:$A$190</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Distribución!$B$40</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Distribución!$B$41:$B$190</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Proporciones!$C$33:$C$42</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Distribución!$A$41:$A$190</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Distribución!$A$193:$A$200</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Distribución!$B$192</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Distribución!$B$193:$B$200</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Distribución!$A$2:$A$37</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Distribución!$B$1</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Distribución!$B$2:$B$37</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Distribución!$C$1</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Distribución!$C$2:$C$37</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Distribución!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Distribución!$C$40</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Distribución!$C$41:$C$190</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Distribución!$D$40</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Distribución!$D$41:$D$190</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Distribución!$A$40</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Distribución!$A$41:$A$190</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Hoja3!$A$1:$A$5</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Hoja3!$B$1:$B$5</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Proporciones!$A$33:$B$42</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Distribución!$B$1</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Distribución!$B$2:$B$37</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Distribución!$C$1</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Distribución!$C$2:$C$37</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Distribución!$A$2:$A$37</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Distribución!$B$1</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Distribución!$B$2:$B$37</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Distribución!$C$1</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Distribución!$C$2:$C$37</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Proporciones!$C$32</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Proporciones!$C$33:$C$42</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Proporciones!$A$33:$B$42</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Proporciones!$C$32</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Proporciones!$C$33:$C$42</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Proporciones!$A$73:$A$82</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Proporciones!$A$73:$A$82</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Proporciones!$B$73:$B$82</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Distribución!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Distribución!$B$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -72,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="44">
   <si>
     <t>Sepal.Length</t>
   </si>
@@ -189,6 +179,21 @@
   </si>
   <si>
     <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Alumnos año anterior</t>
+  </si>
+  <si>
+    <t>Aprobados</t>
+  </si>
+  <si>
+    <t>Nuevas matrículas</t>
+  </si>
+  <si>
+    <t>Abandonan</t>
+  </si>
+  <si>
+    <t>Alumnos en clase</t>
   </si>
 </sst>
 </file>
@@ -5338,6 +5343,13 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -5478,10 +5490,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5491,7 +5503,7 @@
         <cx:series layoutId="sunburst" uniqueId="{22D7E61E-F0FE-4A7C-9F11-49B797FD7217}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>Población</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5533,10 +5545,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.10</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5585,10 +5597,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5598,7 +5610,7 @@
         <cx:series layoutId="treemap" uniqueId="{026EBC8C-2EDA-4897-9223-2D2C5A4CB9D6}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>Población</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5623,18 +5635,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.34</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.36</cx:f>
+        <cx:f>_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.34</cx:f>
+        <cx:f>_xlchart.v1.8</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.38</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5645,7 +5657,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{06A8F964-2F9B-4C6D-ACD7-57AA8E910FF4}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.35</cx:f>
+              <cx:f>_xlchart.v1.9</cx:f>
               <cx:v>Rural</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5658,7 +5670,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{A91A7365-D57D-40AD-B2EB-0C6EF6AF838B}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.37</cx:f>
+              <cx:f>_xlchart.v1.11</cx:f>
               <cx:v>Urbana</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5692,7 +5704,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.20</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5722,7 +5734,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{6412D0C7-A185-4A6F-89AB-8923F4A05303}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.19</cx:f>
+              <cx:f>_xlchart.v1.24</cx:f>
               <cx:v>Sepal.Length</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5756,10 +5768,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5789,7 +5801,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{C898AA8D-C54A-4A46-BDC9-3AB35E4C33F5}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:f>_xlchart.v1.14</cx:f>
               <cx:v>Cantidad</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5827,22 +5839,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.12</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.14</cx:f>
+        <cx:f>_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.16</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.18</cx:f>
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -5872,7 +5884,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{69B1952C-81DB-4BCD-A143-96858D6E7D05}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.11</cx:f>
+              <cx:f>_xlchart.v1.16</cx:f>
               <cx:v>Sepal.Length</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5885,7 +5897,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{20CD4C99-5325-424F-B86B-210292E05602}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.13</cx:f>
+              <cx:f>_xlchart.v1.18</cx:f>
               <cx:v>Sepal.Width</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5898,7 +5910,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F03F70D5-09C7-4A72-9DC7-A75436780008}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.15</cx:f>
+              <cx:f>_xlchart.v1.20</cx:f>
               <cx:v>Petal.Length</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5911,7 +5923,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{F114C8F3-BDCD-43A3-B2B4-09F48BE81A2F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.17</cx:f>
+              <cx:f>_xlchart.v1.22</cx:f>
               <cx:v>Petal.Width</cx:v>
             </cx:txData>
           </cx:tx>
@@ -5932,6 +5944,68 @@
         <cx:tickLabels/>
       </cx:axis>
     </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx8.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.26</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.27</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Alumnos en 2016</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-ES"/>
+            <a:t>Alumnos en 2016</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="waterfall" uniqueId="{4249B9BB-D0D0-4CB8-AFAC-6A6F749AACBD}">
+          <cx:dataLabels pos="outEnd">
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:subtotals>
+              <cx:idx val="4"/>
+            </cx:subtotals>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0.5"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
   </cx:chart>
 </cx:chartSpace>
 </file>
@@ -6174,6 +6248,46 @@
 </file>
 
 <file path=xl/charts/colors15.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -9873,6 +9987,465 @@
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="395">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:bodyPr/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
@@ -14693,6 +15266,83 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>604836</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Gráfico 2"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="604836" y="1133475"/>
+              <a:ext cx="5624513" cy="3619500"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -14958,7 +15608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:D51"/>
     </sheetView>
   </sheetViews>
@@ -18739,7 +19389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D214"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -21280,7 +21930,7 @@
       </c>
       <c r="B193">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -21289,7 +21939,7 @@
       </c>
       <c r="B194">
         <f t="shared" ref="B194:B214" ca="1" si="0">RANDBETWEEN(1,100)</f>
-        <v>2</v>
+        <v>90</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -21298,7 +21948,7 @@
       </c>
       <c r="B195">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>39</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -21307,7 +21957,7 @@
       </c>
       <c r="B196">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>85</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -21316,7 +21966,7 @@
       </c>
       <c r="B197">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -21325,7 +21975,7 @@
       </c>
       <c r="B198">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -21334,7 +21984,7 @@
       </c>
       <c r="B199">
         <f t="shared" ca="1" si="0"/>
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -21352,7 +22002,7 @@
       </c>
       <c r="B201">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -21361,7 +22011,7 @@
       </c>
       <c r="B202">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -21370,7 +22020,7 @@
       </c>
       <c r="B203">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>59</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -21379,7 +22029,7 @@
       </c>
       <c r="B204">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>13</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -21388,7 +22038,7 @@
       </c>
       <c r="B205">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -21397,7 +22047,7 @@
       </c>
       <c r="B206">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -21406,7 +22056,7 @@
       </c>
       <c r="B207">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -21415,7 +22065,7 @@
       </c>
       <c r="B208">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>19</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -21424,7 +22074,7 @@
       </c>
       <c r="B209">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>39</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -21433,7 +22083,7 @@
       </c>
       <c r="B210">
         <f t="shared" ca="1" si="0"/>
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -21442,7 +22092,7 @@
       </c>
       <c r="B211">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -21451,7 +22101,7 @@
       </c>
       <c r="B212">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>89</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -21460,7 +22110,7 @@
       </c>
       <c r="B213">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -21469,7 +22119,67 @@
       </c>
       <c r="B214">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>-128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B1:B4)</f>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hoja con gráfica radial
</commit_message>
<xml_diff>
--- a/08/GraficosII.xlsx
+++ b/08/GraficosII.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Dispersión" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="ColumnasApiladas" sheetId="5" r:id="rId5"/>
     <sheet name="Proporciones" sheetId="6" r:id="rId6"/>
     <sheet name="Distribución" sheetId="7" r:id="rId7"/>
-    <sheet name="Hoja3" sheetId="8" r:id="rId8"/>
+    <sheet name="Cascada" sheetId="8" r:id="rId8"/>
+    <sheet name="Hoja1" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Proporciones!$A$33:$B$42</definedName>
@@ -41,8 +42,8 @@
     <definedName name="_xlchart.v1.23" hidden="1">Distribución!$D$41:$D$190</definedName>
     <definedName name="_xlchart.v1.24" hidden="1">Distribución!$A$40</definedName>
     <definedName name="_xlchart.v1.25" hidden="1">Distribución!$A$41:$A$190</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Hoja3!$A$1:$A$5</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Hoja3!$B$1:$B$5</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Cascada!$A$1:$A$5</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Cascada!$B$1:$B$5</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Proporciones!$A$33:$B$42</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Proporciones!$C$32</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Proporciones!$C$33:$C$42</definedName>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="48">
   <si>
     <t>Sepal.Length</t>
   </si>
@@ -195,6 +196,18 @@
   <si>
     <t>Alumnos en clase</t>
   </si>
+  <si>
+    <t>Activos</t>
+  </si>
+  <si>
+    <t>Ocupados</t>
+  </si>
+  <si>
+    <t>Parados</t>
+  </si>
+  <si>
+    <t>Inactivos</t>
+  </si>
 </sst>
 </file>
 
@@ -267,7 +280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -316,6 +329,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5448,6 +5462,461 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21422194679658754"/>
+          <c:y val="6.2282928919599335E-2"/>
+          <c:w val="0.59418042471947186"/>
+          <c:h val="0.8932915528416091"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2014</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Activos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ocupados</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Inactivos</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Parados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>22954.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17344.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15560</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5610.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-776C-4456-99EA-53F5A96EF3C1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Activos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ocupados</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Inactivos</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Parados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>23364.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18724.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15395.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4640.1000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-776C-4456-99EA-53F5A96EF3C1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2006</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Activos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ocupados</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Inactivos</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Parados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>21780</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19939.099999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15362.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1840.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-776C-4456-99EA-53F5A96EF3C1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="665869512"/>
+        <c:axId val="665871152"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="665869512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="665871152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="665871152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="24000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="665869512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.4275731199835065E-3"/>
+          <c:y val="1.8164872248111842E-2"/>
+          <c:w val="0.22935739829187285"/>
+          <c:h val="3.8265573946113886E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -6327,6 +6796,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -10454,6 +10963,511 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="317">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -15343,6 +16357,41 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -21930,7 +22979,7 @@
       </c>
       <c r="B193">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>83</v>
+        <v>100</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -21939,7 +22988,7 @@
       </c>
       <c r="B194">
         <f t="shared" ref="B194:B214" ca="1" si="0">RANDBETWEEN(1,100)</f>
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -21948,7 +22997,7 @@
       </c>
       <c r="B195">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -21957,7 +23006,7 @@
       </c>
       <c r="B196">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -21966,7 +23015,7 @@
       </c>
       <c r="B197">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -21975,7 +23024,7 @@
       </c>
       <c r="B198">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>20</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -21984,7 +23033,7 @@
       </c>
       <c r="B199">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -21993,7 +23042,7 @@
       </c>
       <c r="B200">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -22002,7 +23051,7 @@
       </c>
       <c r="B201">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -22011,7 +23060,7 @@
       </c>
       <c r="B202">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>62</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -22020,7 +23069,7 @@
       </c>
       <c r="B203">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -22029,7 +23078,7 @@
       </c>
       <c r="B204">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>82</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -22038,7 +23087,7 @@
       </c>
       <c r="B205">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -22047,7 +23096,7 @@
       </c>
       <c r="B206">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -22056,7 +23105,7 @@
       </c>
       <c r="B207">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>20</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -22065,7 +23114,7 @@
       </c>
       <c r="B208">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>51</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -22074,7 +23123,7 @@
       </c>
       <c r="B209">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -22083,7 +23132,7 @@
       </c>
       <c r="B210">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -22092,7 +23141,7 @@
       </c>
       <c r="B211">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -22101,7 +23150,7 @@
       </c>
       <c r="B212">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>42</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -22119,7 +23168,7 @@
       </c>
       <c r="B214">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -22132,8 +23181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -22186,4 +23235,93 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1">
+        <v>2014</v>
+      </c>
+      <c r="C1">
+        <v>2010</v>
+      </c>
+      <c r="D1">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="18">
+        <v>22954.6</v>
+      </c>
+      <c r="C2" s="18">
+        <v>23364.6</v>
+      </c>
+      <c r="D2" s="18">
+        <v>21780</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="18">
+        <v>17344.2</v>
+      </c>
+      <c r="C3" s="18">
+        <v>18724.5</v>
+      </c>
+      <c r="D3" s="18">
+        <v>19939.099999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="18">
+        <v>15560</v>
+      </c>
+      <c r="C4" s="18">
+        <v>15395.5</v>
+      </c>
+      <c r="D4" s="18">
+        <v>15362.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="18">
+        <v>5610.4</v>
+      </c>
+      <c r="C5" s="18">
+        <v>4640.1000000000004</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1840.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Hoja con marcadores de error y línea de tendencia
</commit_message>
<xml_diff>
--- a/08/GraficosII.xlsx
+++ b/08/GraficosII.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43200" windowHeight="20400" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Dispersión" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Proporciones" sheetId="6" r:id="rId6"/>
     <sheet name="Distribución" sheetId="7" r:id="rId7"/>
     <sheet name="Cascada" sheetId="8" r:id="rId8"/>
-    <sheet name="Hoja1" sheetId="9" r:id="rId9"/>
+    <sheet name="Radial" sheetId="9" r:id="rId9"/>
+    <sheet name="Error-Tendencia" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Proporciones!$A$33:$B$42</definedName>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="55">
   <si>
     <t>Sepal.Length</t>
   </si>
@@ -208,12 +209,33 @@
   <si>
     <t>Inactivos</t>
   </si>
+  <si>
+    <t>Temperatura</t>
+  </si>
+  <si>
+    <t>Humedad</t>
+  </si>
+  <si>
+    <t>Visibilidad</t>
+  </si>
+  <si>
+    <t>Día</t>
+  </si>
+  <si>
+    <t>Promedio</t>
+  </si>
+  <si>
+    <t>Rango min</t>
+  </si>
+  <si>
+    <t>Rango max</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +256,12 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -258,7 +286,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -275,12 +303,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDBE1E1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDBE1E1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDBE1E1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDBE1E1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -330,6 +373,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1893,6 +1939,715 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Promedios Jaén enero 2016</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Error-Tendencia'!$B$34:$D$34</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>4.0193548387096758</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>16.193548387096769</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.493548387096773</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Error-Tendencia'!$B$35:$D$35</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.0806451612903238</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>22.806451612903231</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.506451612903227</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Error-Tendencia'!$B$1:$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Temperatura</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Humedad</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Visibilidad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Error-Tendencia'!$B$33:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10.080645161290324</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75.806451612903231</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.506451612903227</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B045-4BD8-A180-C5C7E7C5A95B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="665984048"/>
+        <c:axId val="665989624"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="665984048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="665989624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="665989624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="665984048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Error-Tendencia'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Temperatura</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="34925" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>'Error-Tendencia'!$B$2:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FA48-4444-B20F-A2068691609E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="544012792"/>
+        <c:axId val="544013448"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="544012792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544013448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="544013448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544012792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -5534,7 +6289,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$1</c:f>
+              <c:f>Radial!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5557,7 +6312,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$2:$A$5</c:f>
+              <c:f>Radial!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -5577,7 +6332,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$5</c:f>
+              <c:f>Radial!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -5607,7 +6362,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$1</c:f>
+              <c:f>Radial!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5630,7 +6385,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$2:$A$5</c:f>
+              <c:f>Radial!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -5650,7 +6405,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$5</c:f>
+              <c:f>Radial!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -5680,7 +6435,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$D$1</c:f>
+              <c:f>Radial!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5703,7 +6458,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$A$2:$A$5</c:f>
+              <c:f>Radial!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -5723,7 +6478,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$2:$D$5</c:f>
+              <c:f>Radial!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -6836,6 +7591,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -11472,6 +12307,1012 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style19.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -15528,6 +17369,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -19242,6 +21148,584 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B32" sqref="B1:B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19">
+        <v>13.7</v>
+      </c>
+      <c r="C2" s="19">
+        <v>79</v>
+      </c>
+      <c r="D2" s="19">
+        <v>20</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A3" s="19">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19">
+        <v>11.2</v>
+      </c>
+      <c r="C3" s="19">
+        <v>80</v>
+      </c>
+      <c r="D3" s="19">
+        <v>17.5</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A4" s="19">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19">
+        <v>12</v>
+      </c>
+      <c r="C4" s="19">
+        <v>83</v>
+      </c>
+      <c r="D4" s="19">
+        <v>17.7</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A5" s="19">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19">
+        <v>14.1</v>
+      </c>
+      <c r="C5" s="19">
+        <v>77</v>
+      </c>
+      <c r="D5" s="19">
+        <v>18</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A6" s="19">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19">
+        <v>8.6</v>
+      </c>
+      <c r="C6" s="19">
+        <v>81</v>
+      </c>
+      <c r="D6" s="19">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A7" s="19">
+        <v>6</v>
+      </c>
+      <c r="B7" s="19">
+        <v>7.4</v>
+      </c>
+      <c r="C7" s="19">
+        <v>73</v>
+      </c>
+      <c r="D7" s="19">
+        <v>20</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A8" s="19">
+        <v>7</v>
+      </c>
+      <c r="B8" s="19">
+        <v>12.2</v>
+      </c>
+      <c r="C8" s="19">
+        <v>75</v>
+      </c>
+      <c r="D8" s="19">
+        <v>20</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A9" s="19">
+        <v>8</v>
+      </c>
+      <c r="B9" s="19">
+        <v>12.4</v>
+      </c>
+      <c r="C9" s="19">
+        <v>71</v>
+      </c>
+      <c r="D9" s="19">
+        <v>20</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A10" s="19">
+        <v>9</v>
+      </c>
+      <c r="B10" s="19">
+        <v>12.5</v>
+      </c>
+      <c r="C10" s="19">
+        <v>70</v>
+      </c>
+      <c r="D10" s="19">
+        <v>19.3</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A11" s="19">
+        <v>10</v>
+      </c>
+      <c r="B11" s="19">
+        <v>12.4</v>
+      </c>
+      <c r="C11" s="19">
+        <v>64</v>
+      </c>
+      <c r="D11" s="19">
+        <v>19.8</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A12" s="19">
+        <v>11</v>
+      </c>
+      <c r="B12" s="19">
+        <v>11.1</v>
+      </c>
+      <c r="C12" s="19">
+        <v>79</v>
+      </c>
+      <c r="D12" s="19">
+        <v>15.3</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A13" s="19">
+        <v>12</v>
+      </c>
+      <c r="B13" s="19">
+        <v>8</v>
+      </c>
+      <c r="C13" s="19">
+        <v>76</v>
+      </c>
+      <c r="D13" s="19">
+        <v>19.8</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A14" s="19">
+        <v>13</v>
+      </c>
+      <c r="B14" s="19">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C14" s="19">
+        <v>69</v>
+      </c>
+      <c r="D14" s="19">
+        <v>20</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A15" s="19">
+        <v>14</v>
+      </c>
+      <c r="B15" s="19">
+        <v>9.5</v>
+      </c>
+      <c r="C15" s="19">
+        <v>74</v>
+      </c>
+      <c r="D15" s="19">
+        <v>20</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A16" s="19">
+        <v>15</v>
+      </c>
+      <c r="B16" s="19">
+        <v>9.1</v>
+      </c>
+      <c r="C16" s="19">
+        <v>79</v>
+      </c>
+      <c r="D16" s="19">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A17" s="19">
+        <v>16</v>
+      </c>
+      <c r="B17" s="19">
+        <v>6</v>
+      </c>
+      <c r="C17" s="19">
+        <v>53</v>
+      </c>
+      <c r="D17" s="19">
+        <v>19.8</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A18" s="19">
+        <v>17</v>
+      </c>
+      <c r="B18" s="19">
+        <v>5</v>
+      </c>
+      <c r="C18" s="19">
+        <v>62</v>
+      </c>
+      <c r="D18" s="19">
+        <v>20</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A19" s="19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="19">
+        <v>8.6</v>
+      </c>
+      <c r="C19" s="19">
+        <v>69</v>
+      </c>
+      <c r="D19" s="19">
+        <v>20</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A20" s="19">
+        <v>19</v>
+      </c>
+      <c r="B20" s="19">
+        <v>7.4</v>
+      </c>
+      <c r="C20" s="19">
+        <v>83</v>
+      </c>
+      <c r="D20" s="19">
+        <v>17.2</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A21" s="19">
+        <v>20</v>
+      </c>
+      <c r="B21" s="19">
+        <v>7.5</v>
+      </c>
+      <c r="C21" s="19">
+        <v>92</v>
+      </c>
+      <c r="D21" s="19">
+        <v>14</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A22" s="19">
+        <v>21</v>
+      </c>
+      <c r="B22" s="19">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="C22" s="19">
+        <v>89</v>
+      </c>
+      <c r="D22" s="19">
+        <v>14.3</v>
+      </c>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A23" s="19">
+        <v>22</v>
+      </c>
+      <c r="B23" s="19">
+        <v>11.5</v>
+      </c>
+      <c r="C23" s="19">
+        <v>82</v>
+      </c>
+      <c r="D23" s="19">
+        <v>18.2</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A24" s="19">
+        <v>23</v>
+      </c>
+      <c r="B24" s="19">
+        <v>13.6</v>
+      </c>
+      <c r="C24" s="19">
+        <v>73</v>
+      </c>
+      <c r="D24" s="19">
+        <v>16.7</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A25" s="19">
+        <v>24</v>
+      </c>
+      <c r="B25" s="19">
+        <v>13.7</v>
+      </c>
+      <c r="C25" s="19">
+        <v>70</v>
+      </c>
+      <c r="D25" s="19">
+        <v>20</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A26" s="19">
+        <v>25</v>
+      </c>
+      <c r="B26" s="19">
+        <v>12.5</v>
+      </c>
+      <c r="C26" s="19">
+        <v>72</v>
+      </c>
+      <c r="D26" s="19">
+        <v>20</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A27" s="19">
+        <v>26</v>
+      </c>
+      <c r="B27" s="19">
+        <v>10.7</v>
+      </c>
+      <c r="C27" s="19">
+        <v>79</v>
+      </c>
+      <c r="D27" s="19">
+        <v>19.5</v>
+      </c>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A28" s="19">
+        <v>27</v>
+      </c>
+      <c r="B28" s="19">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C28" s="19">
+        <v>78</v>
+      </c>
+      <c r="D28" s="19">
+        <v>19.3</v>
+      </c>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A29" s="19">
+        <v>28</v>
+      </c>
+      <c r="B29" s="19">
+        <v>9.1</v>
+      </c>
+      <c r="C29" s="19">
+        <v>74</v>
+      </c>
+      <c r="D29" s="19">
+        <v>19.5</v>
+      </c>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A30" s="19">
+        <v>29</v>
+      </c>
+      <c r="B30" s="19">
+        <v>9</v>
+      </c>
+      <c r="C30" s="19">
+        <v>80</v>
+      </c>
+      <c r="D30" s="19">
+        <v>18.5</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A31" s="19">
+        <v>30</v>
+      </c>
+      <c r="B31" s="19">
+        <v>8.6</v>
+      </c>
+      <c r="C31" s="19">
+        <v>85</v>
+      </c>
+      <c r="D31" s="19">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A32" s="19">
+        <v>31</v>
+      </c>
+      <c r="B32" s="19">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C32" s="19">
+        <v>79</v>
+      </c>
+      <c r="D32" s="19">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33">
+        <f>AVERAGE(B2:B32)</f>
+        <v>10.080645161290324</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:D33" si="0">AVERAGE(C2:C32)</f>
+        <v>75.806451612903231</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>18.506451612903227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34">
+        <f>MAX(B2:B32)-B33</f>
+        <v>4.0193548387096758</v>
+      </c>
+      <c r="C34">
+        <f>MAX(C2:C32)-C33</f>
+        <v>16.193548387096769</v>
+      </c>
+      <c r="D34">
+        <f>MAX(D2:D32)-D33</f>
+        <v>1.493548387096773</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35">
+        <f>B33-MIN(B2:B32)</f>
+        <v>5.0806451612903238</v>
+      </c>
+      <c r="C35">
+        <f>C33-MIN(C2:C32)</f>
+        <v>22.806451612903231</v>
+      </c>
+      <c r="D35">
+        <f>D33-MIN(D2:D32)</f>
+        <v>4.506451612903227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
@@ -22979,7 +25463,7 @@
       </c>
       <c r="B193">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>100</v>
+        <v>44</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -22988,7 +25472,7 @@
       </c>
       <c r="B194">
         <f t="shared" ref="B194:B214" ca="1" si="0">RANDBETWEEN(1,100)</f>
-        <v>88</v>
+        <v>30</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -22997,7 +25481,7 @@
       </c>
       <c r="B195">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -23006,7 +25490,7 @@
       </c>
       <c r="B196">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -23015,7 +25499,7 @@
       </c>
       <c r="B197">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>97</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -23024,7 +25508,7 @@
       </c>
       <c r="B198">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>85</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -23033,7 +25517,7 @@
       </c>
       <c r="B199">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>16</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -23042,7 +25526,7 @@
       </c>
       <c r="B200">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>64</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -23051,7 +25535,7 @@
       </c>
       <c r="B201">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>75</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -23060,7 +25544,7 @@
       </c>
       <c r="B202">
         <f t="shared" ca="1" si="0"/>
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -23069,7 +25553,7 @@
       </c>
       <c r="B203">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>100</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -23078,7 +25562,7 @@
       </c>
       <c r="B204">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -23087,7 +25571,7 @@
       </c>
       <c r="B205">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>33</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -23096,7 +25580,7 @@
       </c>
       <c r="B206">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -23105,7 +25589,7 @@
       </c>
       <c r="B207">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>75</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -23114,7 +25598,7 @@
       </c>
       <c r="B208">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>84</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -23123,7 +25607,7 @@
       </c>
       <c r="B209">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>63</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -23132,7 +25616,7 @@
       </c>
       <c r="B210">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>16</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -23141,7 +25625,7 @@
       </c>
       <c r="B211">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>36</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -23150,7 +25634,7 @@
       </c>
       <c r="B212">
         <f t="shared" ca="1" si="0"/>
-        <v>42</v>
+        <v>5</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -23159,7 +25643,7 @@
       </c>
       <c r="B213">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -23168,7 +25652,7 @@
       </c>
       <c r="B214">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -23241,7 +25725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>